<commit_message>
Fix sheet removed from spreadsheet
</commit_message>
<xml_diff>
--- a/PHORCYS/data/raw/Iselin_WHOI_2016_11/Iselin_WHOI_2016_11_Winklers.xlsx
+++ b/PHORCYS/data/raw/Iselin_WHOI_2016_11/Iselin_WHOI_2016_11_Winklers.xlsx
@@ -1,18 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/DO_Instruments/PHORCYS/data/raw/Iselin_WHOI_2016_11/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="15135" windowHeight="7875" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21540" windowHeight="16020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="110816" sheetId="1" r:id="rId1"/>
     <sheet name="110916" sheetId="2" r:id="rId2"/>
     <sheet name="111016" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="111116" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" refMode="R1C1"/>
+  <calcPr calcId="124519" refMode="R1C1" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -292,11 +305,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +361,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -394,12 +412,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -426,14 +444,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -460,6 +479,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,14 +655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,7 +740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,7 +922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,14 +1084,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1273,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1325,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1377,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1429,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1455,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1481,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1487,7 +1507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1513,7 +1533,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1559,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1611,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1637,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1663,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,16 +1721,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1788,7 +1808,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1834,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1860,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1886,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1892,7 +1912,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1944,7 +1964,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1970,7 +1990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +2016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +2068,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2100,7 +2120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +2146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2172,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2198,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2204,7 +2224,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2250,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2256,7 +2276,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2282,7 +2302,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2308,7 +2328,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2341,16 +2361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E24"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2376,7 +2396,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2402,7 +2422,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2428,7 +2448,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2454,7 +2474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2480,7 +2500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2506,7 +2526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2532,7 +2552,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2558,7 +2578,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2610,7 +2630,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2636,7 +2656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2662,7 +2682,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2688,7 +2708,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2734,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2760,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2766,7 +2786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +2812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2818,7 +2838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2844,7 +2864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2870,7 +2890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2896,7 +2916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2922,7 +2942,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2948,7 +2968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>